<commit_message>
Tuned up the other two scenarios, for now
</commit_message>
<xml_diff>
--- a/Output/Tuning_Sims/TuningSimsComparison.xlsx
+++ b/Output/Tuning_Sims/TuningSimsComparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtstevens/Documents/New Mexico/USGS/Research/Swiss Cheese/Conchas_High_Severity/Output/Tuning_Sims/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C889A7BF-680E-874C-A7FB-AC792F837716}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3FDFA0-EBAF-6E43-A763-E2E44DCF6C81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="460" windowWidth="26740" windowHeight="15880" activeTab="5" xr2:uid="{57C99E8A-1D76-B348-B2CB-5D1E92DB10D4}"/>
+    <workbookView xWindow="1940" yWindow="460" windowWidth="26740" windowHeight="15880" activeTab="6" xr2:uid="{57C99E8A-1D76-B348-B2CB-5D1E92DB10D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Beta2" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Beta5" sheetId="7" r:id="rId4"/>
     <sheet name="Beta6" sheetId="8" r:id="rId5"/>
     <sheet name="Alpha1" sheetId="10" r:id="rId6"/>
+    <sheet name="Theta1" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="68">
   <si>
     <t>nugget</t>
   </si>
@@ -228,6 +229,21 @@
   </si>
   <si>
     <t>Going with this one.</t>
+  </si>
+  <si>
+    <t>We pull two different ranges of the Gaussian field</t>
+  </si>
+  <si>
+    <t>1-18% + &gt;71%</t>
+  </si>
+  <si>
+    <t>1-18% + &gt;50%</t>
+  </si>
+  <si>
+    <t>2-18% + &gt;50</t>
+  </si>
+  <si>
+    <t>1-19% + &gt;50</t>
   </si>
 </sst>
 </file>
@@ -280,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -288,6 +304,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1859,7 +1877,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-      <selection pane="bottomRight" sqref="A1:I2"/>
+      <selection pane="bottomRight" sqref="A1:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1899,35 +1917,38 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="5">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="E2" s="5">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="C3">
         <v>0.5</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>0.5</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C3">
-        <v>0.75</v>
-      </c>
-      <c r="D3">
-        <v>0.75</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -1935,8 +1956,12 @@
       <c r="F3" t="s">
         <v>55</v>
       </c>
-      <c r="H3">
-        <v>1.1000000000000001</v>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1944,19 +1969,19 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="3">
-        <v>2</v>
+        <v>55</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1973,10 +1998,10 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1987,17 +2012,16 @@
         <v>0.5</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="3"/>
+        <v>60</v>
+      </c>
       <c r="H6" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2008,20 +2032,17 @@
         <v>0.5</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3">
-        <v>5</v>
-      </c>
-      <c r="I7" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -2029,7 +2050,7 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -2042,31 +2063,31 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
       <c r="B9">
         <v>0.35399999999999998</v>
       </c>
       <c r="C9">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2074,23 +2095,19 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>0.75</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>55</v>
+      </c>
       <c r="H10" s="3">
-        <v>8</v>
-      </c>
-      <c r="I10" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -2098,10 +2115,10 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -2111,7 +2128,7 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -2119,7 +2136,7 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>0.25</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2132,7 +2149,7 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -2140,10 +2157,10 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -2153,19 +2170,21 @@
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="I13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
       <c r="B14">
         <v>0.35399999999999998</v>
       </c>
       <c r="C14">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -2175,7 +2194,7 @@
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2183,61 +2202,90 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="C15">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
         <v>52</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" t="s">
-        <v>58</v>
+      <c r="H15" s="3">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>0.35399999999999998</v>
+      </c>
       <c r="C16">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D16">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17">
+        <v>0.35399999999999998</v>
+      </c>
       <c r="C17">
-        <v>0.75</v>
+        <v>20</v>
       </c>
       <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="C18">
         <v>0.5</v>
       </c>
-      <c r="E17">
-        <v>10</v>
-      </c>
-      <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="3">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>51</v>
       </c>
@@ -2254,11 +2302,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717F0AAA-72D2-F34F-8505-1200220EF437}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2299,7 +2347,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="5">
-        <v>0.35399999999999998</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="C2" s="5">
         <v>0.6</v>
@@ -2311,7 +2359,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="6">
@@ -2322,353 +2370,65 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C3">
-        <v>0.5</v>
-      </c>
-      <c r="D3">
-        <v>0.5</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>55</v>
-      </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="3">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C4">
-        <v>0.75</v>
-      </c>
-      <c r="D4">
-        <v>0.75</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
+      <c r="H3" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C5">
-        <v>0.5</v>
-      </c>
-      <c r="D5">
-        <v>0.5</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="3">
-        <v>4</v>
-      </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C6">
-        <v>0.5</v>
-      </c>
-      <c r="D6">
-        <v>0.5</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="3">
-        <v>5</v>
-      </c>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C7">
-        <v>0.5</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>55</v>
-      </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="3">
-        <v>6</v>
-      </c>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C8">
-        <v>0.5</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="3">
-        <v>7</v>
-      </c>
-      <c r="I8" t="s">
-        <v>54</v>
-      </c>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C9">
-        <v>0.5</v>
-      </c>
-      <c r="D9">
-        <v>0.75</v>
-      </c>
-      <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>55</v>
-      </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="3">
-        <v>8</v>
-      </c>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C10">
-        <v>0.75</v>
-      </c>
-      <c r="D10">
-        <v>0.5</v>
-      </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="3">
-        <v>9</v>
-      </c>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="3">
-        <v>10</v>
-      </c>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C12">
-        <v>0.25</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>52</v>
-      </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="3">
-        <v>11</v>
-      </c>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>52</v>
-      </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="3">
-        <v>12</v>
-      </c>
-      <c r="I13" t="s">
-        <v>53</v>
-      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>52</v>
-      </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="3">
-        <v>13</v>
-      </c>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>10</v>
-      </c>
-      <c r="F15" t="s">
-        <v>52</v>
-      </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="3">
-        <v>14</v>
-      </c>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16" t="s">
-        <v>52</v>
-      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
-      <c r="B17">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C17">
-        <v>20</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>10</v>
-      </c>
-      <c r="F17" t="s">
-        <v>52</v>
-      </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B18">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="C18">
-        <v>0.5</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>20</v>
-      </c>
-      <c r="F18" t="s">
-        <v>52</v>
-      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G18" s="3"/>
-      <c r="H18" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2677,4 +2437,230 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0FD621-A8C4-6947-98F8-4C386894CCE0}">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B2:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B2" s="7">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>0.3</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="7">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="7">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="7">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="7">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="7">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="7">
+        <v>10</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G18" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I7">
+    <sortCondition ref="H1:H7"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Further edits ahead of presentation on 2/18/21 (finalize simulations, EDA figures, etc).
</commit_message>
<xml_diff>
--- a/Output/Tuning_Sims/TuningSimsComparison.xlsx
+++ b/Output/Tuning_Sims/TuningSimsComparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtstevens/Documents/New Mexico/USGS/Research/Swiss Cheese/Conchas_High_Severity/Output/Tuning_Sims/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3FDFA0-EBAF-6E43-A763-E2E44DCF6C81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB7AEEF-B2B3-0B4D-B7C7-35BB7DE2BE1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="460" windowWidth="26740" windowHeight="15880" activeTab="6" xr2:uid="{57C99E8A-1D76-B348-B2CB-5D1E92DB10D4}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="26740" windowHeight="15880" activeTab="4" xr2:uid="{57C99E8A-1D76-B348-B2CB-5D1E92DB10D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Beta2" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="69">
   <si>
     <t>nugget</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>1-19% + &gt;50</t>
+  </si>
+  <si>
+    <t>This was the version that created the January GIF</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1101,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1373,6 +1376,11 @@
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I14" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
@@ -1873,11 +1881,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABE28C3-92A5-0240-BF55-1BBA8A4EF2C8}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-      <selection pane="bottomRight" sqref="A1:L22"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2283,6 +2291,23 @@
       </c>
       <c r="I18" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>0.25</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19">
+        <v>11.5</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2443,7 +2468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0FD621-A8C4-6947-98F8-4C386894CCE0}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>

</xml_diff>